<commit_message>
Added results for multi-qubit fidelity
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14020" windowWidth="21820" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14020" windowWidth="21820" xWindow="-110" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="Porter_Thomas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Two_qubit_fidelity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Multi_qubit_fidelity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" refMode="R1C1"/>
@@ -85451,7 +85452,7 @@
   </sheetPr>
   <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -87860,4 +87861,1373 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.9999999999999996</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.9999999999999998</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.9999999999999999</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.9999999999999998</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0.9999999999999999</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.9999999999999991</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.9999999999999996</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0.9975284716977462</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.9638618187874645</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.9999999999999998</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0.9886388454407095</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.9351702982086929</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.9980287268179067</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.9728927079794467</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.9999999999999998</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.9999999999999991</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0.9898317349735312</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.8446391903463212</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.9968024855988438</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.9559309917503636</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.9994706760021338</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.9976980298759844</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0.9752778774485117</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.6797298850561199</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.996178515245844</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.9069514829111364</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.9994810045450907</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.9935039869289917</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0.9793585488446043</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.4997808913296969</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.9924240007316799</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.8835650196835112</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.9985340266494855</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.9787215325688144</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0.9595926891965265</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.3309510964961775</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.9898427624885022</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.8102793873831907</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.9984598640292467</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.9626687784873917</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0.9569784556804083</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.24057316209785204</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.9789524027752247</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.7010148922266324</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.9965240211542609</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.926573427869234</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0.9233610115943023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.15216240754849636</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.9667113270674282</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.5952018560085253</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.9951811776189005</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.9005494853333628</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0.9444920724405748</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0.08689283163200259</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.9847098442774307</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.4285015225520468</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0.9920057082791969</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0.8661874063983098</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0.9282494870049126</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0.055702880937660196</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.9641259888566899</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.3595366099450983</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0.9877736275722708</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0.817292399559428</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0.9436563314576419</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0.03675471545489852</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.9662342440704986</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.23980954858793668</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0.986461127199691</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0.7219821447283694</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0.9437942349767552</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.01905986532157093</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.9559262716045202</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.19271425781866994</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0.9856306450608191</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0.660323788453426</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0.932750600935691</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.012178680423484928</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.9602689606768</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.12780697154610726</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.9820735828226811</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0.55432353372269</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0.9358548658681284</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0.006342587645911301</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.9675735621164506</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.09012089206928639</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.9735773302212589</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0.5061099111436245</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0.9378564886355464</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.004239419577894983</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.9639240011424405</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.06465502716798047</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.9810189881824312</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0.41539892347103013</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0.947577661695712</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.0023039257039833495</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.9451615182325646</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.04659471910179421</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.9795135843340975</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0.3404802474106149</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0.9380232610630282</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0.0012348000468564593</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.9600414049450341</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.031596485932728326</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.9682638940481276</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0.26482609037987626</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0.9381841340426768</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.000584313636456046</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.9637391505047291</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.02075789254381546</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.9845981615245205</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0.20661586783339625</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0.9379540709207703</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0.0003859948893576825</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.9646936240892926</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.014013221050685504</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.966818487963842</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0.16838602122445884</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0.9332787530591284</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.00022350476698166467</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.9706278109850908</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.009470060404444761</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0.9712022836852451</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0.12047195409154157</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0.9456431931321851</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.000131351230917407</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.9743212240703274</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.006384432808249788</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.9705174357018557</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0.08869614487003318</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0.9441062250730744</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>7.474895266518346e-05</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.9566798774864592</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.004101749378490087</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0.9487582662460302</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>3.789046155974221e-05</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.9712621987827051</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.0027668462661666537</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0.9249656829146858</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2.7412970444028004e-05</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0.9513517469039859</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.0018655497037977533</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0.933282441431512</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1.861121578886998e-05</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0.9647551627081123</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.0011137849128783509</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0.9336898090504143</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1.0119273068577818e-05</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.9542376917583547</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.0007428216115198193</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0.9426443473547501</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1.115755948796743e-05</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.9630758465041722</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.00040489026530680916</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0.9444895264879868</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>4.1321242158652866e-06</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.9508294525941141</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.0002441542661199678</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0.9408895838427395</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2.1420345069005633e-06</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.9594518100013029</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.00015726918759493668</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>0.9291996948318093</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>5.078482219863495e-06</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.9482578711806148</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>8.548426837186698e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0.9590866750507065</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>4.458532235532586e-06</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0.9648647682165917</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>5.536343341494502e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0.9366034227621188</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2.1502647877915326e-06</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.9670206113983673</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2.3550338224417508e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0.9505919810170279</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1.7812273055186353e-06</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.9583038545147248</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1.4045074089349634e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0.9099030499953744</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>7.844469463225438e-07</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.9586479369127683</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>8.167610419351914e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0.9552456676086443</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1.2040415531779482e-06</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.9579954807400195</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7.2369687035348445e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0.9337243671909122</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1.0166942654508274e-07</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.9649651689795758</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>8.039775332109232e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>0.9517759566033444</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>4.9892300091114114e-06</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0.9678765441729926</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>9.202078131289957e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0.9398401428286413</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>3.404004836572968e-06</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0.9631047556049804</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>3.885100070422563e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>0.946190174891669</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1.3233895622277472e-06</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0.9617277298127936</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>4.321388599904069e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>0.9347172999646729</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2.582298725781132e-07</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.9673216096637237</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2.8666808434095752e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0.9402610767692726</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1.8618509288570674e-07</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.9565116473132251</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>1.9491412147595098e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0.9413203493723766</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>8.027484336539393e-08</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.9689006658976205</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1.3697626422234069e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0.9363302582951751</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1.0912883757892506e-06</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.9544088866841088</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>4.872141896653974e-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>0.9251761184383428</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1.277790491093836e-06</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0.956241726707407</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1.5711523110528523e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>0.9480978453950172</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>8.450937189286067e-07</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.9625595216463121</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2.895788350463419e-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>0.9318701395874858</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>5.273613983788518e-07</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0.9478193435603651</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>6.326773890466455e-07</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added and tested ortonormalization of tt-cores, but only using truncated SVD instead of QR
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14020" windowWidth="21820" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14020" windowWidth="21820" xWindow="-110" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="Porter_Thomas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Two_qubit_fidelity" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Multi_qubit_fidelity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Two_qubit_fidelity_qr" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" refMode="R1C1"/>
@@ -87871,7 +87872,7 @@
   </sheetPr>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -89230,4 +89231,626 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="26.36328125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1.0000000000000009</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.9999999999999999</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1.000000000000001</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.9999999999999998</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.999999290915343</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1.0000000000000004</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.9999999743143172</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1.0000000000000013</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.9999999658987833</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1.0000000000000002</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.9999997903604043</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0.9999999999999493</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0.9998169594755374</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0.9999999999917378</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0.9994065768094089</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0.9999999998482394</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0.9994928953257465</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0.9999999985595687</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.9989415365157558</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0.999999980763129</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.9985053377069114</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0.9999999043783523</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0.9979798208448912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0.999999389523212</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.9973744596850095</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0.9999981072081476</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.9961477583016676</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0.9999895615189962</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0.9957750716636464</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0.9999842251110351</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.995866529223471</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0.9999479723079016</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0.9919711296210081</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0.9999007828345382</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.9943580450641126</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0.9998630083926582</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.9898790855290649</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0.9996821138171678</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.9920125516720569</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0.9995936000984884</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0.9915725561138936</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0.9995296440888338</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0.9836141818651124</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0.9989229427229451</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0.9908075109930113</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0.9993162758845977</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0.9868741559321801</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0.9986935531120037</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0.985416406761039</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0.9984524403223033</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>0.9879336631288052</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0.9972358043083257</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0.9878699318631081</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>0.9977938678843631</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>0.9856414401299113</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0.9969300953266369</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>0.9830609581608041</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0.9972807257180839</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0.9832845915769173</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0.9966674212484908</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0.9859715426232848</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0.9953752306929141</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0.9808587754592127</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0.9954711998908878</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0.9810847941371186</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0.9959609672297567</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0.9844240234078806</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>0.9946782808311575</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0.9856505950843946</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0.993474760600469</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0.9876413486448731</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>0.9943355791816457</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0.9803659349751512</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>0.9913087686581581</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0.9858408142236056</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0.9933239447545619</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0.9841016981079742</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0.9902258130646006</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0.9831507882661265</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0.9919740122106124</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0.9831912916297157</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>0.9919091758884668</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0.9806467599638503</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>0.9923611159221776</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0.9798722784311096</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>0.9917694910118453</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0.978621743064091</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>